<commit_message>
separation graph crypto stocks
</commit_message>
<xml_diff>
--- a/cryptos_market_cap.xlsx
+++ b/cryptos_market_cap.xlsx
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>578604019979.7795</v>
+        <v>658635213881.7474</v>
       </c>
     </row>
     <row r="3">
@@ -477,7 +477,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>192935713287.9787</v>
+        <v>213648463155.1176</v>
       </c>
     </row>
     <row r="4">
@@ -492,7 +492,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>84197413447.3663</v>
+        <v>84291615051.44429</v>
       </c>
     </row>
     <row r="5">
@@ -507,7 +507,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>32201997216.81027</v>
+        <v>34149224073.46932</v>
       </c>
     </row>
     <row r="6">
@@ -522,7 +522,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>27511566886.78043</v>
+        <v>29763354750.16835</v>
       </c>
     </row>
     <row r="7">
@@ -537,7 +537,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>25535798696.84357</v>
+        <v>25147785370.52747</v>
       </c>
     </row>
     <row r="8">
@@ -552,7 +552,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>11203658469.09467</v>
+        <v>12810329657.90201</v>
       </c>
     </row>
     <row r="9">
@@ -567,7 +567,7 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>8854891899.827383</v>
+        <v>9795719791.685951</v>
       </c>
     </row>
     <row r="10">
@@ -582,7 +582,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>8479425903.814398</v>
+        <v>9346057965.164358</v>
       </c>
     </row>
     <row r="11">
@@ -597,7 +597,7 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>8071139607.940892</v>
+        <v>8190902529.1807</v>
       </c>
     </row>
     <row r="12">
@@ -612,37 +612,37 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>7135310392.814843</v>
+        <v>7335984498.418167</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Dai</t>
+          <t>Polygon</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>DAI-USD</t>
+          <t>MATIC-USD</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>5348728900.169457</v>
+        <v>5842193209.048368</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Polygon</t>
+          <t>Chainlink</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>MATIC-USD</t>
+          <t>LINK-USD</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>5001681884.497235</v>
+        <v>5555046571.631498</v>
       </c>
     </row>
     <row r="15">
@@ -657,22 +657,22 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>4835413385.104083</v>
+        <v>5502141881.324093</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Polkadot</t>
+          <t>Dai</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>DOT-USD</t>
+          <t>DAI-USD</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>4806976383.729829</v>
+        <v>5346266803.592254</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
separation graph crypto stocks 2.0
</commit_message>
<xml_diff>
--- a/cryptos_market_cap.xlsx
+++ b/cryptos_market_cap.xlsx
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>658635213881.7474</v>
+        <v>658352313258.7543</v>
       </c>
     </row>
     <row r="3">
@@ -477,7 +477,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>213648463155.1176</v>
+        <v>213442894232.639</v>
       </c>
     </row>
     <row r="4">
@@ -492,7 +492,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>84291615051.44429</v>
+        <v>84286479133.81744</v>
       </c>
     </row>
     <row r="5">
@@ -507,7 +507,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>34149224073.46932</v>
+        <v>34164644572.66166</v>
       </c>
     </row>
     <row r="6">
@@ -522,7 +522,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>29763354750.16835</v>
+        <v>29854210078.56976</v>
       </c>
     </row>
     <row r="7">
@@ -537,7 +537,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>25147785370.52747</v>
+        <v>25147468736.90444</v>
       </c>
     </row>
     <row r="8">
@@ -552,7 +552,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>12810329657.90201</v>
+        <v>12822792468.38154</v>
       </c>
     </row>
     <row r="9">
@@ -567,7 +567,7 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>9795719791.685951</v>
+        <v>9809135720.351103</v>
       </c>
     </row>
     <row r="10">
@@ -582,7 +582,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>9346057965.164358</v>
+        <v>9356571675.282593</v>
       </c>
     </row>
     <row r="11">
@@ -597,7 +597,7 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>8190902529.1807</v>
+        <v>8193279980.061813</v>
       </c>
     </row>
     <row r="12">
@@ -612,7 +612,7 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>7335984498.418167</v>
+        <v>7339386720.365101</v>
       </c>
     </row>
     <row r="13">
@@ -627,7 +627,7 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>5842193209.048368</v>
+        <v>5842478283.745811</v>
       </c>
     </row>
     <row r="14">
@@ -642,7 +642,7 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>5555046571.631498</v>
+        <v>5559553646.899556</v>
       </c>
     </row>
     <row r="15">
@@ -657,7 +657,7 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>5502141881.324093</v>
+        <v>5502725656.295998</v>
       </c>
     </row>
     <row r="16">
@@ -672,7 +672,7 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>5346266803.592254</v>
+        <v>5346120983.163179</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add input and portfolio repartition
</commit_message>
<xml_diff>
--- a/cryptos_market_cap.xlsx
+++ b/cryptos_market_cap.xlsx
@@ -58,16 +58,16 @@
     <t>Toncoin</t>
   </si>
   <si>
+    <t>Chainlink</t>
+  </si>
+  <si>
     <t>Polygon</t>
   </si>
   <si>
-    <t>Chainlink</t>
-  </si>
-  <si>
     <t>Wrapped Bitcoin</t>
   </si>
   <si>
-    <t>Dai</t>
+    <t>Polkadot</t>
   </si>
   <si>
     <t>BTC-USD</t>
@@ -103,16 +103,16 @@
     <t>TON-USD</t>
   </si>
   <si>
+    <t>LINK-USD</t>
+  </si>
+  <si>
     <t>MATIC-USD</t>
   </si>
   <si>
-    <t>LINK-USD</t>
-  </si>
-  <si>
     <t>WBTC-USD</t>
   </si>
   <si>
-    <t>DAI-USD</t>
+    <t>DOT-USD</t>
   </si>
 </sst>
 </file>
@@ -495,7 +495,7 @@
         <v>18</v>
       </c>
       <c r="C2">
-        <v>662153919805.8962</v>
+        <v>667481036535.8472</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -506,7 +506,7 @@
         <v>19</v>
       </c>
       <c r="C3">
-        <v>214670624083.8028</v>
+        <v>216164763891.7112</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -517,7 +517,7 @@
         <v>20</v>
       </c>
       <c r="C4">
-        <v>84297525672.00328</v>
+        <v>84284224915.32452</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -528,7 +528,7 @@
         <v>21</v>
       </c>
       <c r="C5">
-        <v>34283990582.80655</v>
+        <v>34610024098.47021</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -539,7 +539,7 @@
         <v>22</v>
       </c>
       <c r="C6">
-        <v>29898981363.4091</v>
+        <v>29816346122.12012</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -550,7 +550,7 @@
         <v>23</v>
       </c>
       <c r="C7">
-        <v>25086252129.6169</v>
+        <v>25092265828.22784</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -561,7 +561,7 @@
         <v>24</v>
       </c>
       <c r="C8">
-        <v>12624958104.41818</v>
+        <v>13280642821.8183</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -572,7 +572,7 @@
         <v>25</v>
       </c>
       <c r="C9">
-        <v>9843473977.850145</v>
+        <v>9994479857.705906</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -583,7 +583,7 @@
         <v>26</v>
       </c>
       <c r="C10">
-        <v>9435354260.451193</v>
+        <v>9473857229.459873</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -594,7 +594,7 @@
         <v>27</v>
       </c>
       <c r="C11">
-        <v>8202753618.690736</v>
+        <v>8240592331.9852</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -605,7 +605,7 @@
         <v>28</v>
       </c>
       <c r="C12">
-        <v>7306042720.390573</v>
+        <v>7353642028.759882</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -616,7 +616,7 @@
         <v>29</v>
       </c>
       <c r="C13">
-        <v>5820807342.399495</v>
+        <v>6278567002.412182</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -627,7 +627,7 @@
         <v>30</v>
       </c>
       <c r="C14">
-        <v>5783482676.888522</v>
+        <v>5914919560.103052</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -638,7 +638,7 @@
         <v>31</v>
       </c>
       <c r="C15">
-        <v>5574112092.889112</v>
+        <v>5600297319.235932</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -649,7 +649,7 @@
         <v>32</v>
       </c>
       <c r="C16">
-        <v>5345451533.691011</v>
+        <v>5552575781.656272</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
PF distribution Not fixed ! NEED SOME CHANGE
</commit_message>
<xml_diff>
--- a/cryptos_market_cap.xlsx
+++ b/cryptos_market_cap.xlsx
@@ -495,7 +495,7 @@
         <v>18</v>
       </c>
       <c r="C2">
-        <v>667481036535.8472</v>
+        <v>666663244656.6726</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -506,7 +506,7 @@
         <v>19</v>
       </c>
       <c r="C3">
-        <v>216164763891.7112</v>
+        <v>215894388530.8438</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -517,7 +517,7 @@
         <v>20</v>
       </c>
       <c r="C4">
-        <v>84284224915.32452</v>
+        <v>84259407156.79712</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -528,7 +528,7 @@
         <v>21</v>
       </c>
       <c r="C5">
-        <v>34610024098.47021</v>
+        <v>34490373188.7056</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -539,7 +539,7 @@
         <v>22</v>
       </c>
       <c r="C6">
-        <v>29816346122.12012</v>
+        <v>29812930074.87981</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -550,7 +550,7 @@
         <v>23</v>
       </c>
       <c r="C7">
-        <v>25092265828.22784</v>
+        <v>25079116536.25563</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -561,7 +561,7 @@
         <v>24</v>
       </c>
       <c r="C8">
-        <v>13280642821.8183</v>
+        <v>13075337557.07294</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -572,7 +572,7 @@
         <v>25</v>
       </c>
       <c r="C9">
-        <v>9994479857.705906</v>
+        <v>9938396539.221432</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -583,7 +583,7 @@
         <v>26</v>
       </c>
       <c r="C10">
-        <v>9473857229.459873</v>
+        <v>9414554630.551594</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -594,7 +594,7 @@
         <v>27</v>
       </c>
       <c r="C11">
-        <v>8240592331.9852</v>
+        <v>8233547006.034203</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -605,7 +605,7 @@
         <v>28</v>
       </c>
       <c r="C12">
-        <v>7353642028.759882</v>
+        <v>7345088469.253864</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -616,7 +616,7 @@
         <v>29</v>
       </c>
       <c r="C13">
-        <v>6278567002.412182</v>
+        <v>6362933528.338446</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -627,7 +627,7 @@
         <v>30</v>
       </c>
       <c r="C14">
-        <v>5914919560.103052</v>
+        <v>5941956028.061554</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -638,7 +638,7 @@
         <v>31</v>
       </c>
       <c r="C15">
-        <v>5600297319.235932</v>
+        <v>5606911520.500404</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -649,7 +649,7 @@
         <v>32</v>
       </c>
       <c r="C16">
-        <v>5552575781.656272</v>
+        <v>5548924012.004469</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New env and import
</commit_message>
<xml_diff>
--- a/cryptos_market_cap.xlsx
+++ b/cryptos_market_cap.xlsx
@@ -67,7 +67,7 @@
     <t>Wrapped Bitcoin</t>
   </si>
   <si>
-    <t>Polkadot</t>
+    <t>Dai</t>
   </si>
   <si>
     <t>BTC-USD</t>
@@ -112,7 +112,7 @@
     <t>WBTC-USD</t>
   </si>
   <si>
-    <t>DOT-USD</t>
+    <t>DAI-USD</t>
   </si>
 </sst>
 </file>
@@ -495,7 +495,7 @@
         <v>18</v>
       </c>
       <c r="C2">
-        <v>666663244656.6726</v>
+        <v>667110329317.8585</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -506,7 +506,7 @@
         <v>19</v>
       </c>
       <c r="C3">
-        <v>215894388530.8438</v>
+        <v>215741838217.8916</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -517,7 +517,7 @@
         <v>20</v>
       </c>
       <c r="C4">
-        <v>84259407156.79712</v>
+        <v>84537893987.737</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -528,7 +528,7 @@
         <v>21</v>
       </c>
       <c r="C5">
-        <v>34490373188.7056</v>
+        <v>34701356782.98159</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -539,7 +539,7 @@
         <v>22</v>
       </c>
       <c r="C6">
-        <v>29812930074.87981</v>
+        <v>29596095256.35921</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -550,7 +550,7 @@
         <v>23</v>
       </c>
       <c r="C7">
-        <v>25079116536.25563</v>
+        <v>25098292739.90195</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -561,7 +561,7 @@
         <v>24</v>
       </c>
       <c r="C8">
-        <v>13075337557.07294</v>
+        <v>13760373926.07715</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -572,7 +572,7 @@
         <v>25</v>
       </c>
       <c r="C9">
-        <v>9938396539.221432</v>
+        <v>10211926471.06009</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -583,7 +583,7 @@
         <v>26</v>
       </c>
       <c r="C10">
-        <v>9414554630.551594</v>
+        <v>10141885921.13766</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -594,7 +594,7 @@
         <v>27</v>
       </c>
       <c r="C11">
-        <v>8233547006.034203</v>
+        <v>8327370113.840555</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -605,7 +605,7 @@
         <v>28</v>
       </c>
       <c r="C12">
-        <v>7345088469.253864</v>
+        <v>7169555497.918983</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -616,7 +616,7 @@
         <v>29</v>
       </c>
       <c r="C13">
-        <v>6362933528.338446</v>
+        <v>6217803225.309694</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -627,7 +627,7 @@
         <v>30</v>
       </c>
       <c r="C14">
-        <v>5941956028.061554</v>
+        <v>5833348926.360915</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -638,7 +638,7 @@
         <v>31</v>
       </c>
       <c r="C15">
-        <v>5606911520.500404</v>
+        <v>5592650380.386826</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -649,7 +649,7 @@
         <v>32</v>
       </c>
       <c r="C16">
-        <v>5548924012.004469</v>
+        <v>5348447881.94701</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refacto is ok !
</commit_message>
<xml_diff>
--- a/cryptos_market_cap.xlsx
+++ b/cryptos_market_cap.xlsx
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>714580396488.1063</v>
+        <v>707764416716.2303</v>
       </c>
     </row>
     <row r="3">
@@ -477,7 +477,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>246177523190.341</v>
+        <v>241861615405.5887</v>
       </c>
     </row>
     <row r="4">
@@ -492,7 +492,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>87116031200.74547</v>
+        <v>87347430651.04588</v>
       </c>
     </row>
     <row r="5">
@@ -507,7 +507,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>37410286527.14858</v>
+        <v>37376344664.52251</v>
       </c>
     </row>
     <row r="6">
@@ -522,37 +522,37 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>35398108612.24805</v>
+        <v>34322046171.68675</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>USDC</t>
+          <t>Solana</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>USDC-USD</t>
+          <t>SOL-USD</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>24023558993.11394</v>
+        <v>26604916001.90222</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Solana</t>
+          <t>USDC</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>SOL-USD</t>
+          <t>USDC-USD</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>23301455943.60514</v>
+        <v>23931425825.1214</v>
       </c>
     </row>
     <row r="9">
@@ -567,7 +567,7 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>12918342440.65112</v>
+        <v>13037134434.13486</v>
       </c>
     </row>
     <row r="10">
@@ -582,7 +582,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>10583769483.99507</v>
+        <v>10583343498.86235</v>
       </c>
     </row>
     <row r="11">
@@ -597,7 +597,7 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>9392119720.793606</v>
+        <v>9261916358.333483</v>
       </c>
     </row>
     <row r="12">
@@ -612,7 +612,7 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>8792621553.59626</v>
+        <v>8763528480.611448</v>
       </c>
     </row>
     <row r="13">
@@ -627,7 +627,7 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>8096914969.536195</v>
+        <v>8318387938.914449</v>
       </c>
     </row>
     <row r="14">
@@ -642,37 +642,37 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>8087721301.526255</v>
+        <v>7889662081.524138</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Polkadot</t>
+          <t>Avalanche</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>DOT-USD</t>
+          <t>AVAX-USD</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>6768882186.68738</v>
+        <v>6959721541.2058</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Avalanche</t>
+          <t>Polkadot</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>AVAX-USD</t>
+          <t>DOT-USD</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>6146855809.299229</v>
+        <v>6774478471.431178</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More crypto asset and efficient line is ok !
</commit_message>
<xml_diff>
--- a/cryptos_market_cap.xlsx
+++ b/cryptos_market_cap.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>707764416716.2303</v>
+        <v>708479008611.6012</v>
       </c>
     </row>
     <row r="3">
@@ -477,202 +477,352 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>241861615405.5887</v>
+        <v>242091520445.6097</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Tether USDt</t>
+          <t>BNB</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>USDT-USD</t>
+          <t>BNB-USD</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>87347430651.04588</v>
+        <v>38255025955.62946</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>BNB</t>
+          <t>XRP</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>BNB-USD</t>
+          <t>XRP-USD</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>37376344664.52251</v>
+        <v>34204919250.52261</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>XRP</t>
+          <t>Solana</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>XRP-USD</t>
+          <t>SOL-USD</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>34322046171.68675</v>
+        <v>26411865956.14902</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Solana</t>
+          <t>Cardano</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>SOL-USD</t>
+          <t>ADA-USD</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>26604916001.90222</v>
+        <v>13006021840.74045</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>USDC</t>
+          <t>Dogecoin</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>USDC-USD</t>
+          <t>DOGE-USD</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>23931425825.1214</v>
+        <v>10523736344.92889</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Cardano</t>
+          <t>TRON</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>ADA-USD</t>
+          <t>TRX-USD</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>13037134434.13486</v>
+        <v>9236740082.654627</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Dogecoin</t>
+          <t>Polygon</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>DOGE-USD</t>
+          <t>MATIC-USD</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>10583343498.86235</v>
+        <v>8378001144.125881</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>TRON</t>
+          <t>Chainlink</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>TRX-USD</t>
+          <t>LINK-USD</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>9261916358.333483</v>
+        <v>8218904526.219995</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Polygon</t>
+          <t>Toncoin</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>MATIC-USD</t>
+          <t>TON-USD</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>8763528480.611448</v>
+        <v>7867658202.653782</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Chainlink</t>
+          <t>Avalanche</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>LINK-USD</t>
+          <t>AVAX-USD</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>8318387938.914449</v>
+        <v>7018185773.453343</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Toncoin</t>
+          <t>Polkadot</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>TON-USD</t>
+          <t>DOT-USD</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>7889662081.524138</v>
+        <v>6752494904.928741</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Avalanche</t>
+          <t>Wrapped Bitcoin</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>AVAX-USD</t>
+          <t>WBTC-USD</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>6959721541.2058</v>
+        <v>5922102614.900625</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Polkadot</t>
+          <t>Litecoin</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>DOT-USD</t>
+          <t>LTC-USD</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>6774478471.431178</v>
+        <v>5318515548.766405</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Shiba Inu</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>SHIB-USD</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>5059433485.511156</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Bitcoin Cash</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>BCH-USD</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>4556617892.441616</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>UNUS SED LEO</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>LEO-USD</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>3707281230.704166</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Cosmos</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>ATOM-USD</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>3575037140.071479</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>OKB</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>OKB-USD</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>3561330600.496291</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Stellar</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>XLM-USD</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>3356540063.866071</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Monero</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>XMR-USD</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>3000328346.07416</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Ethereum Classic</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>ETC-USD</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>2795690272.088627</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Cronos</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>CRO-USD</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>2563723725.813462</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Kaspa</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>KAS-USD</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>2514361673.708901</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ajout excel file with zone bourse data
</commit_message>
<xml_diff>
--- a/cryptos_market_cap.xlsx
+++ b/cryptos_market_cap.xlsx
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>708479008611.6012</v>
+        <v>712204551721.0481</v>
       </c>
     </row>
     <row r="3">
@@ -477,7 +477,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>242091520445.6097</v>
+        <v>242724325270.2232</v>
       </c>
     </row>
     <row r="4">
@@ -492,7 +492,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>38255025955.62946</v>
+        <v>38347168320.21263</v>
       </c>
     </row>
     <row r="5">
@@ -507,7 +507,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>34204919250.52261</v>
+        <v>34385820455.79092</v>
       </c>
     </row>
     <row r="6">
@@ -522,7 +522,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>26411865956.14902</v>
+        <v>26538465526.84064</v>
       </c>
     </row>
     <row r="7">
@@ -537,7 +537,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>13006021840.74045</v>
+        <v>13131836977.62074</v>
       </c>
     </row>
     <row r="8">
@@ -552,7 +552,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>10523736344.92889</v>
+        <v>10570140100.82911</v>
       </c>
     </row>
     <row r="9">
@@ -567,7 +567,7 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>9236740082.654627</v>
+        <v>9249568473.746784</v>
       </c>
     </row>
     <row r="10">
@@ -582,7 +582,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>8378001144.125881</v>
+        <v>8465833466.668921</v>
       </c>
     </row>
     <row r="11">
@@ -597,7 +597,7 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>8218904526.219995</v>
+        <v>8301810750.139015</v>
       </c>
     </row>
     <row r="12">
@@ -612,7 +612,7 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>7867658202.653782</v>
+        <v>7961214387.485915</v>
       </c>
     </row>
     <row r="13">
@@ -627,7 +627,7 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>7018185773.453343</v>
+        <v>7217284884.089936</v>
       </c>
     </row>
     <row r="14">
@@ -642,7 +642,7 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>6752494904.928741</v>
+        <v>6794857449.435575</v>
       </c>
     </row>
     <row r="15">
@@ -657,7 +657,7 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>5922102614.900625</v>
+        <v>5954412669.867033</v>
       </c>
     </row>
     <row r="16">
@@ -672,7 +672,7 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>5318515548.766405</v>
+        <v>5340065056.106133</v>
       </c>
     </row>
     <row r="17">
@@ -687,7 +687,7 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>5059433485.511156</v>
+        <v>5094964998.879547</v>
       </c>
     </row>
     <row r="18">
@@ -702,7 +702,7 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>4556617892.441616</v>
+        <v>4571873154.264347</v>
       </c>
     </row>
     <row r="19">
@@ -717,7 +717,7 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>3707281230.704166</v>
+        <v>3768600131.609521</v>
       </c>
     </row>
     <row r="20">
@@ -732,7 +732,7 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>3575037140.071479</v>
+        <v>3614769306.166145</v>
       </c>
     </row>
     <row r="21">
@@ -747,7 +747,7 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>3561330600.496291</v>
+        <v>3580676608.937095</v>
       </c>
     </row>
     <row r="22">
@@ -762,7 +762,7 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>3356540063.866071</v>
+        <v>3373783328.34027</v>
       </c>
     </row>
     <row r="23">
@@ -777,7 +777,7 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>3000328346.07416</v>
+        <v>3009527136.437813</v>
       </c>
     </row>
     <row r="24">
@@ -792,7 +792,7 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>2795690272.088627</v>
+        <v>2805664665.719321</v>
       </c>
     </row>
     <row r="25">
@@ -807,7 +807,7 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>2563723725.813462</v>
+        <v>2602614942.655396</v>
       </c>
     </row>
     <row r="26">
@@ -822,7 +822,7 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>2514361673.708901</v>
+        <v>2499993416.47157</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Survey + recommend portfolio (not finished)
</commit_message>
<xml_diff>
--- a/cryptos_market_cap.xlsx
+++ b/cryptos_market_cap.xlsx
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>733006206290.2766</v>
+        <v>737133302290.2677</v>
       </c>
     </row>
     <row r="3">
@@ -477,7 +477,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>246027458445.7996</v>
+        <v>247244493778.9961</v>
       </c>
     </row>
     <row r="4">
@@ -492,7 +492,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>38288155320.38718</v>
+        <v>38390659845.19044</v>
       </c>
     </row>
     <row r="5">
@@ -507,7 +507,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>34550736489.83262</v>
+        <v>34685910398.30289</v>
       </c>
     </row>
     <row r="6">
@@ -522,7 +522,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>27983153894.43178</v>
+        <v>27532074178.23908</v>
       </c>
     </row>
     <row r="7">
@@ -537,7 +537,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>13258735176.62395</v>
+        <v>13393577812.97504</v>
       </c>
     </row>
     <row r="8">
@@ -552,7 +552,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>10677601142.78642</v>
+        <v>10819894707.74953</v>
       </c>
     </row>
     <row r="9">
@@ -567,37 +567,37 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>9186857589.440948</v>
+        <v>9242314400.824749</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Chainlink</t>
+          <t>Polygon</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>LINK-USD</t>
+          <t>MATIC-USD</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>8443581512.366194</v>
+        <v>8507732893.082836</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Polygon</t>
+          <t>Chainlink</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>MATIC-USD</t>
+          <t>LINK-USD</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>8428675931.057423</v>
+        <v>8325744672.079366</v>
       </c>
     </row>
     <row r="12">
@@ -612,7 +612,7 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>8116098098.534303</v>
+        <v>8189957692.931383</v>
       </c>
     </row>
     <row r="13">
@@ -627,7 +627,7 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>7356541480.021262</v>
+        <v>7354641270.491064</v>
       </c>
     </row>
     <row r="14">
@@ -642,7 +642,7 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>7002337482.612908</v>
+        <v>6982621694.335486</v>
       </c>
     </row>
     <row r="15">
@@ -657,7 +657,7 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>6142891204.468773</v>
+        <v>6178344669.330246</v>
       </c>
     </row>
     <row r="16">
@@ -672,7 +672,7 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>5434967706.614725</v>
+        <v>5463567574.120149</v>
       </c>
     </row>
     <row r="17">
@@ -687,7 +687,7 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>5176951328.968423</v>
+        <v>5176763885.483999</v>
       </c>
     </row>
     <row r="18">
@@ -702,7 +702,7 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>4621781663.473914</v>
+        <v>4682341026.782693</v>
       </c>
     </row>
     <row r="19">
@@ -717,7 +717,7 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>3774590863.917698</v>
+        <v>3777671236.637238</v>
       </c>
     </row>
     <row r="20">
@@ -732,7 +732,7 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>3594864910.98273</v>
+        <v>3648354300.80387</v>
       </c>
     </row>
     <row r="21">
@@ -747,7 +747,7 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>3592408650.38277</v>
+        <v>3614419588.569764</v>
       </c>
     </row>
     <row r="22">
@@ -762,7 +762,7 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>3389512290.447855</v>
+        <v>3398722194.285174</v>
       </c>
     </row>
     <row r="23">
@@ -777,7 +777,7 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>3040998226.731361</v>
+        <v>2979199919.429708</v>
       </c>
     </row>
     <row r="24">
@@ -792,7 +792,7 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>2837087455.626977</v>
+        <v>2856082645.519599</v>
       </c>
     </row>
     <row r="25">
@@ -807,7 +807,7 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>2589439101.553806</v>
+        <v>2624592537.812566</v>
       </c>
     </row>
     <row r="26">
@@ -822,7 +822,7 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>2471166048.952417</v>
+        <v>2522164756.451115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Stocks names and cryptos names
</commit_message>
<xml_diff>
--- a/cryptos_market_cap.xlsx
+++ b/cryptos_market_cap.xlsx
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>737133302290.2677</v>
+        <v>719536829972.2048</v>
       </c>
     </row>
     <row r="3">
@@ -477,7 +477,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>247244493778.9961</v>
+        <v>244206525520.8783</v>
       </c>
     </row>
     <row r="4">
@@ -492,7 +492,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>38390659845.19044</v>
+        <v>37859945782.87637</v>
       </c>
     </row>
     <row r="5">
@@ -507,7 +507,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>34685910398.30289</v>
+        <v>33915828443.44218</v>
       </c>
     </row>
     <row r="6">
@@ -522,7 +522,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>27532074178.23908</v>
+        <v>26526553149.50745</v>
       </c>
     </row>
     <row r="7">
@@ -537,7 +537,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>13393577812.97504</v>
+        <v>13824714680.37449</v>
       </c>
     </row>
     <row r="8">
@@ -552,7 +552,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>10819894707.74953</v>
+        <v>11189935570.81735</v>
       </c>
     </row>
     <row r="9">
@@ -567,37 +567,37 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>9242314400.824749</v>
+        <v>9165671380.355772</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Polygon</t>
+          <t>Avalanche</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>MATIC-USD</t>
+          <t>AVAX-USD</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>8507732893.082836</v>
+        <v>8293800081.851548</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Chainlink</t>
+          <t>Polygon</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>LINK-USD</t>
+          <t>MATIC-USD</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>8325744672.079366</v>
+        <v>8283365709.063359</v>
       </c>
     </row>
     <row r="12">
@@ -612,22 +612,22 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>8189957692.931383</v>
+        <v>8010828924.011144</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Avalanche</t>
+          <t>Chainlink</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>AVAX-USD</t>
+          <t>LINK-USD</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>7354641270.491064</v>
+        <v>7985886591.259349</v>
       </c>
     </row>
     <row r="14">
@@ -642,7 +642,7 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>6982621694.335486</v>
+        <v>7060867585.842254</v>
       </c>
     </row>
     <row r="15">
@@ -657,7 +657,7 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>6178344669.330246</v>
+        <v>6018844475.097538</v>
       </c>
     </row>
     <row r="16">
@@ -672,7 +672,7 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>5463567574.120149</v>
+        <v>5360223441.43322</v>
       </c>
     </row>
     <row r="17">
@@ -687,7 +687,7 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>5176763885.483999</v>
+        <v>5221139601.473591</v>
       </c>
     </row>
     <row r="18">
@@ -702,7 +702,7 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>4682341026.782693</v>
+        <v>4596806846.195675</v>
       </c>
     </row>
     <row r="19">
@@ -717,37 +717,37 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>3777671236.637238</v>
+        <v>3750487646.599951</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>OKB</t>
+          <t>Cosmos</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>OKB-USD</t>
+          <t>ATOM-USD</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>3648354300.80387</v>
+        <v>3715654109.491059</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Cosmos</t>
+          <t>OKB</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>ATOM-USD</t>
+          <t>OKB-USD</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>3614419588.569764</v>
+        <v>3523067013.188245</v>
       </c>
     </row>
     <row r="22">
@@ -762,67 +762,67 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>3398722194.285174</v>
+        <v>3377547916.808996</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Monero</t>
+          <t>Kaspa</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>XMR-USD</t>
+          <t>KAS-USD</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>2979199919.429708</v>
+        <v>3001318881.208693</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Ethereum Classic</t>
+          <t>Monero</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>ETC-USD</t>
+          <t>XMR-USD</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>2856082645.519599</v>
+        <v>2946760695.065717</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Cronos</t>
+          <t>Ethereum Classic</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>CRO-USD</t>
+          <t>ETC-USD</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>2624592537.812566</v>
+        <v>2876157252.276538</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Filecoin</t>
+          <t>Cronos</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>FIL-USD</t>
+          <t>CRO-USD</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>2522164756.451115</v>
+        <v>2513593377.987969</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Stocks names and cryptos names PRT2
</commit_message>
<xml_diff>
--- a/cryptos_market_cap.xlsx
+++ b/cryptos_market_cap.xlsx
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>719536829972.2048</v>
+        <v>721202497449.1852</v>
       </c>
     </row>
     <row r="3">
@@ -477,7 +477,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>244206525520.8783</v>
+        <v>244685368352.3357</v>
       </c>
     </row>
     <row r="4">
@@ -492,7 +492,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>37859945782.87637</v>
+        <v>37832035877.15541</v>
       </c>
     </row>
     <row r="5">
@@ -507,7 +507,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>33915828443.44218</v>
+        <v>33930139813.33422</v>
       </c>
     </row>
     <row r="6">
@@ -522,7 +522,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>26526553149.50745</v>
+        <v>26502594024.89571</v>
       </c>
     </row>
     <row r="7">
@@ -537,7 +537,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>13824714680.37449</v>
+        <v>13932760853.96851</v>
       </c>
     </row>
     <row r="8">
@@ -552,7 +552,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>11189935570.81735</v>
+        <v>11143606318.32923</v>
       </c>
     </row>
     <row r="9">
@@ -567,37 +567,37 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>9165671380.355772</v>
+        <v>9172445970.432299</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Avalanche</t>
+          <t>Polygon</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>AVAX-USD</t>
+          <t>MATIC-USD</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>8293800081.851548</v>
+        <v>8288439414.011463</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Polygon</t>
+          <t>Avalanche</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>MATIC-USD</t>
+          <t>AVAX-USD</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>8283365709.063359</v>
+        <v>8286989881.493361</v>
       </c>
     </row>
     <row r="12">
@@ -612,7 +612,7 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>8010828924.011144</v>
+        <v>8057833605.645318</v>
       </c>
     </row>
     <row r="13">
@@ -627,7 +627,7 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>7985886591.259349</v>
+        <v>8005791334.873327</v>
       </c>
     </row>
     <row r="14">
@@ -642,7 +642,7 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>7060867585.842254</v>
+        <v>7089270478.055191</v>
       </c>
     </row>
     <row r="15">
@@ -657,7 +657,7 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>6018844475.097538</v>
+        <v>6024677236.291335</v>
       </c>
     </row>
     <row r="16">
@@ -672,7 +672,7 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>5360223441.43322</v>
+        <v>5363446399.970418</v>
       </c>
     </row>
     <row r="17">
@@ -687,7 +687,7 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>5221139601.473591</v>
+        <v>5206001255.311966</v>
       </c>
     </row>
     <row r="18">
@@ -702,7 +702,7 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>4596806846.195675</v>
+        <v>4595203878.57365</v>
       </c>
     </row>
     <row r="19">
@@ -717,7 +717,7 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>3750487646.599951</v>
+        <v>3719839375.908229</v>
       </c>
     </row>
     <row r="20">
@@ -732,7 +732,7 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>3715654109.491059</v>
+        <v>3706033919.912179</v>
       </c>
     </row>
     <row r="21">
@@ -747,7 +747,7 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>3523067013.188245</v>
+        <v>3521926218.888741</v>
       </c>
     </row>
     <row r="22">
@@ -762,7 +762,7 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>3377547916.808996</v>
+        <v>3383257432.909583</v>
       </c>
     </row>
     <row r="23">
@@ -777,7 +777,7 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>3001318881.208693</v>
+        <v>3017812634.355353</v>
       </c>
     </row>
     <row r="24">
@@ -792,7 +792,7 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>2946760695.065717</v>
+        <v>2951921492.128325</v>
       </c>
     </row>
     <row r="25">
@@ -807,7 +807,7 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>2876157252.276538</v>
+        <v>2881111534.018945</v>
       </c>
     </row>
     <row r="26">
@@ -822,7 +822,7 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>2513593377.987969</v>
+        <v>2525262868.699377</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ajout rathio de sharp
</commit_message>
<xml_diff>
--- a/cryptos_market_cap.xlsx
+++ b/cryptos_market_cap.xlsx
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>721202497449.1852</v>
+        <v>713688901027.9006</v>
       </c>
     </row>
     <row r="3">
@@ -477,7 +477,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>244685368352.3357</v>
+        <v>240904302203.1317</v>
       </c>
     </row>
     <row r="4">
@@ -492,7 +492,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>37832035877.15541</v>
+        <v>37421036288.88834</v>
       </c>
     </row>
     <row r="5">
@@ -507,7 +507,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>33930139813.33422</v>
+        <v>33516769668.61184</v>
       </c>
     </row>
     <row r="6">
@@ -522,7 +522,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>26502594024.89571</v>
+        <v>25941175676.57832</v>
       </c>
     </row>
     <row r="7">
@@ -537,7 +537,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>13932760853.96851</v>
+        <v>13491724901.42055</v>
       </c>
     </row>
     <row r="8">
@@ -552,7 +552,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>11143606318.32923</v>
+        <v>10948878600.2546</v>
       </c>
     </row>
     <row r="9">
@@ -567,7 +567,7 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>9172445970.432299</v>
+        <v>9133398904.990887</v>
       </c>
     </row>
     <row r="10">
@@ -582,7 +582,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>8288439414.011463</v>
+        <v>8162374780.375494</v>
       </c>
     </row>
     <row r="11">
@@ -597,7 +597,7 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>8286989881.493361</v>
+        <v>8110987920.436409</v>
       </c>
     </row>
     <row r="12">
@@ -612,7 +612,7 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>8057833605.645318</v>
+        <v>7935764574.283823</v>
       </c>
     </row>
     <row r="13">
@@ -627,7 +627,7 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>8005791334.873327</v>
+        <v>7888159434.931012</v>
       </c>
     </row>
     <row r="14">
@@ -642,7 +642,7 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>7089270478.055191</v>
+        <v>7004567269.532668</v>
       </c>
     </row>
     <row r="15">
@@ -657,7 +657,7 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>6024677236.291335</v>
+        <v>5970710377.514452</v>
       </c>
     </row>
     <row r="16">
@@ -672,7 +672,7 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>5363446399.970418</v>
+        <v>5305017541.105283</v>
       </c>
     </row>
     <row r="17">
@@ -687,7 +687,7 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>5206001255.311966</v>
+        <v>5127623626.674</v>
       </c>
     </row>
     <row r="18">
@@ -702,7 +702,7 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>4595203878.57365</v>
+        <v>4542817292.301433</v>
       </c>
     </row>
     <row r="19">
@@ -717,7 +717,7 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>3719839375.908229</v>
+        <v>3760213762.134553</v>
       </c>
     </row>
     <row r="20">
@@ -732,7 +732,7 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>3706033919.912179</v>
+        <v>3664101041.967874</v>
       </c>
     </row>
     <row r="21">
@@ -747,7 +747,7 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>3521926218.888741</v>
+        <v>3485833767.538836</v>
       </c>
     </row>
     <row r="22">
@@ -762,7 +762,7 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>3383257432.909583</v>
+        <v>3351316873.553715</v>
       </c>
     </row>
     <row r="23">
@@ -777,7 +777,7 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>3017812634.355353</v>
+        <v>2964508064.322744</v>
       </c>
     </row>
     <row r="24">
@@ -792,7 +792,7 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>2951921492.128325</v>
+        <v>2928518666.515219</v>
       </c>
     </row>
     <row r="25">
@@ -807,7 +807,7 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>2881111534.018945</v>
+        <v>2835973127.381089</v>
       </c>
     </row>
     <row r="26">
@@ -822,7 +822,7 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>2525262868.699377</v>
+        <v>2482378317.382869</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Try to add the PE Ratio
</commit_message>
<xml_diff>
--- a/cryptos_market_cap.xlsx
+++ b/cryptos_market_cap.xlsx
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>707906016350.917</v>
+        <v>709599331094.9697</v>
       </c>
     </row>
     <row r="3">
@@ -477,7 +477,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>238576545449.2376</v>
+        <v>232009741643.4652</v>
       </c>
     </row>
     <row r="4">
@@ -492,7 +492,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>37161313028.19727</v>
+        <v>36763362405.97121</v>
       </c>
     </row>
     <row r="5">
@@ -507,7 +507,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>33327875606.73561</v>
+        <v>32303492845.14954</v>
       </c>
     </row>
     <row r="6">
@@ -522,7 +522,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>26128119273.39835</v>
+        <v>23863430866.82423</v>
       </c>
     </row>
     <row r="7">
@@ -537,7 +537,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>13335097921.62567</v>
+        <v>12826871086.8618</v>
       </c>
     </row>
     <row r="8">
@@ -552,7 +552,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>11220108590.26807</v>
+        <v>11677096606.99001</v>
       </c>
     </row>
     <row r="9">
@@ -567,37 +567,37 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>9111227859.364193</v>
+        <v>9088763660.586021</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Polygon</t>
+          <t>Toncoin</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>MATIC-USD</t>
+          <t>TON-USD</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>8035719462.267957</v>
+        <v>7814775280.991043</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Toncoin</t>
+          <t>Polygon</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>TON-USD</t>
+          <t>MATIC-USD</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>7981389751.144408</v>
+        <v>7539009532.292098</v>
       </c>
     </row>
     <row r="12">
@@ -612,7 +612,7 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>7913296108.926406</v>
+        <v>7533781949.363321</v>
       </c>
     </row>
     <row r="13">
@@ -627,7 +627,7 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>7790295317.02891</v>
+        <v>7408357493.749443</v>
       </c>
     </row>
     <row r="14">
@@ -642,7 +642,7 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>6869144465.276965</v>
+        <v>6602397511.290756</v>
       </c>
     </row>
     <row r="15">
@@ -657,7 +657,7 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>5930543393.709435</v>
+        <v>5958607945.875978</v>
       </c>
     </row>
     <row r="16">
@@ -672,7 +672,7 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>5260794442.867391</v>
+        <v>5111727373.900389</v>
       </c>
     </row>
     <row r="17">
@@ -687,7 +687,7 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>5114274252.125801</v>
+        <v>5062042475.280413</v>
       </c>
     </row>
     <row r="18">
@@ -702,7 +702,7 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>4590289469.593143</v>
+        <v>4431124989.914836</v>
       </c>
     </row>
     <row r="19">
@@ -717,7 +717,7 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>3746615946.852252</v>
+        <v>3770368267.006455</v>
       </c>
     </row>
     <row r="20">
@@ -732,7 +732,7 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>3697893509.232855</v>
+        <v>3456637581.265154</v>
       </c>
     </row>
     <row r="21">
@@ -747,7 +747,7 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>3432385330.672878</v>
+        <v>3350340934.019464</v>
       </c>
     </row>
     <row r="22">
@@ -762,52 +762,52 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>3338026702.59357</v>
+        <v>3259399994.280393</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Kaspa</t>
+          <t>Monero</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>KAS-USD</t>
+          <t>XMR-USD</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>2932777445.059374</v>
+        <v>2984873211.79517</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Monero</t>
+          <t>Ethereum Classic</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>XMR-USD</t>
+          <t>ETC-USD</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>2932102011.75055</v>
+        <v>2726804834.093751</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Ethereum Classic</t>
+          <t>Kaspa</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>ETC-USD</t>
+          <t>KAS-USD</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>2814100955.769952</v>
+        <v>2634899949.649961</v>
       </c>
     </row>
     <row r="26">
@@ -822,7 +822,7 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>2457346526.566064</v>
+        <v>2427815139.415774</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
mise en place ploting
</commit_message>
<xml_diff>
--- a/cryptos_market_cap.xlsx
+++ b/cryptos_market_cap.xlsx
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>727683411616.0249</v>
+        <v>730781075708.5688</v>
       </c>
     </row>
     <row r="3">
@@ -477,7 +477,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>243512160780.3604</v>
+        <v>245257091704.5142</v>
       </c>
     </row>
     <row r="4">
@@ -492,7 +492,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>37541233480.68076</v>
+        <v>37558555657.86328</v>
       </c>
     </row>
     <row r="5">
@@ -507,7 +507,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>33539494594.78046</v>
+        <v>33331957411.70317</v>
       </c>
     </row>
     <row r="6">
@@ -522,7 +522,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>25578497759.71209</v>
+        <v>25311182965.7804</v>
       </c>
     </row>
     <row r="7">
@@ -537,7 +537,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>13770658592.77569</v>
+        <v>13828792225.42868</v>
       </c>
     </row>
     <row r="8">
@@ -552,7 +552,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>11530518436.7949</v>
+        <v>11456884589.16068</v>
       </c>
     </row>
     <row r="9">
@@ -567,7 +567,7 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>9268992390.106615</v>
+        <v>9235860793.291689</v>
       </c>
     </row>
     <row r="10">
@@ -582,7 +582,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>8399549448.9212</v>
+        <v>8453209150.625892</v>
       </c>
     </row>
     <row r="11">
@@ -597,7 +597,7 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>8094113995.839714</v>
+        <v>8111096848.791776</v>
       </c>
     </row>
     <row r="12">
@@ -612,7 +612,7 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>7892452774.591537</v>
+        <v>7869724955.00743</v>
       </c>
     </row>
     <row r="13">
@@ -627,7 +627,7 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>7778373822.380466</v>
+        <v>7842322201.283567</v>
       </c>
     </row>
     <row r="14">
@@ -642,7 +642,7 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>6830600606.39605</v>
+        <v>6816510736.856397</v>
       </c>
     </row>
     <row r="15">
@@ -657,7 +657,7 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>6074129892.491833</v>
+        <v>6082869313.002133</v>
       </c>
     </row>
     <row r="16">
@@ -672,7 +672,7 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>5207497463.269599</v>
+        <v>5208165229.352201</v>
       </c>
     </row>
     <row r="17">
@@ -687,7 +687,7 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>5112146593.72781</v>
+        <v>5077501592.809649</v>
       </c>
     </row>
     <row r="18">
@@ -702,7 +702,7 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>4489172894.021282</v>
+        <v>4482371364.744591</v>
       </c>
     </row>
     <row r="19">
@@ -717,7 +717,7 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>3663655073.672228</v>
+        <v>3661721163.844837</v>
       </c>
     </row>
     <row r="20">
@@ -732,7 +732,7 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>3527963882.813667</v>
+        <v>3520144110.326622</v>
       </c>
     </row>
     <row r="21">
@@ -747,7 +747,7 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>3453450705.229949</v>
+        <v>3482261875.863487</v>
       </c>
     </row>
     <row r="22">
@@ -762,7 +762,7 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>3385864700.635701</v>
+        <v>3395851447.907824</v>
       </c>
     </row>
     <row r="23">
@@ -777,7 +777,7 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>3009523107.433399</v>
+        <v>3021454679.573148</v>
       </c>
     </row>
     <row r="24">
@@ -792,7 +792,7 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>3001668198.498478</v>
+        <v>2940131061.636749</v>
       </c>
     </row>
     <row r="25">
@@ -807,7 +807,7 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>2825101983.516402</v>
+        <v>2851678189.604074</v>
       </c>
     </row>
     <row r="26">
@@ -822,7 +822,7 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>2458337702.181116</v>
+        <v>2446990549.970589</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
mise en place survey
</commit_message>
<xml_diff>
--- a/cryptos_market_cap.xlsx
+++ b/cryptos_market_cap.xlsx
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>730781075708.5688</v>
+        <v>734020108300.9487</v>
       </c>
     </row>
     <row r="3">
@@ -477,7 +477,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>245257091704.5142</v>
+        <v>246066347323.4598</v>
       </c>
     </row>
     <row r="4">
@@ -492,7 +492,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>37558555657.86328</v>
+        <v>38992486587.04223</v>
       </c>
     </row>
     <row r="5">
@@ -507,7 +507,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>33331957411.70317</v>
+        <v>33307298629.42934</v>
       </c>
     </row>
     <row r="6">
@@ -522,7 +522,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>25311182965.7804</v>
+        <v>24253458545.67005</v>
       </c>
     </row>
     <row r="7">
@@ -537,7 +537,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>13828792225.42868</v>
+        <v>13677197642.06798</v>
       </c>
     </row>
     <row r="8">
@@ -552,7 +552,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>11456884589.16068</v>
+        <v>11359429835.55813</v>
       </c>
     </row>
     <row r="9">
@@ -567,7 +567,7 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>9235860793.291689</v>
+        <v>9119366109.749874</v>
       </c>
     </row>
     <row r="10">
@@ -582,7 +582,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>8453209150.625892</v>
+        <v>8257079728.487464</v>
       </c>
     </row>
     <row r="11">
@@ -597,7 +597,7 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>8111096848.791776</v>
+        <v>8093285119.901435</v>
       </c>
     </row>
     <row r="12">
@@ -612,7 +612,7 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>7869724955.00743</v>
+        <v>7637931566.491719</v>
       </c>
     </row>
     <row r="13">
@@ -627,7 +627,7 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>7842322201.283567</v>
+        <v>7592349038.162902</v>
       </c>
     </row>
     <row r="14">
@@ -642,7 +642,7 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>6816510736.856397</v>
+        <v>6727678885.928888</v>
       </c>
     </row>
     <row r="15">
@@ -657,7 +657,7 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>6082869313.002133</v>
+        <v>6131783021.903178</v>
       </c>
     </row>
     <row r="16">
@@ -672,7 +672,7 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>5208165229.352201</v>
+        <v>5185208942.700999</v>
       </c>
     </row>
     <row r="17">
@@ -687,7 +687,7 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>5077501592.809649</v>
+        <v>5060123103.839664</v>
       </c>
     </row>
     <row r="18">
@@ -702,7 +702,7 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>4482371364.744591</v>
+        <v>4467550118.133206</v>
       </c>
     </row>
     <row r="19">
@@ -717,37 +717,37 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>3661721163.844837</v>
+        <v>3651225093.29196</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Cosmos</t>
+          <t>OKB</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>ATOM-USD</t>
+          <t>OKB-USD</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>3520144110.326622</v>
+        <v>3454728662.767564</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>OKB</t>
+          <t>Cosmos</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>OKB-USD</t>
+          <t>ATOM-USD</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>3482261875.863487</v>
+        <v>3453696439.300338</v>
       </c>
     </row>
     <row r="22">
@@ -762,37 +762,37 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>3395851447.907824</v>
+        <v>3366126614.056954</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Monero</t>
+          <t>Kaspa</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>XMR-USD</t>
+          <t>KAS-USD</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>3021454679.573148</v>
+        <v>3015161535.871074</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Kaspa</t>
+          <t>Monero</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>KAS-USD</t>
+          <t>XMR-USD</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>2940131061.636749</v>
+        <v>3004347745.952567</v>
       </c>
     </row>
     <row r="25">
@@ -807,7 +807,7 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>2851678189.604074</v>
+        <v>2841200082.369965</v>
       </c>
     </row>
     <row r="26">
@@ -822,7 +822,7 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>2446990549.970589</v>
+        <v>2440675830.95558</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
plot sharp best weight
</commit_message>
<xml_diff>
--- a/cryptos_market_cap.xlsx
+++ b/cryptos_market_cap.xlsx
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>736618623046.0665</v>
+        <v>734283209566.5956</v>
       </c>
     </row>
     <row r="3">
@@ -477,7 +477,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>245831843180.7638</v>
+        <v>245227573040.3853</v>
       </c>
     </row>
     <row r="4">
@@ -492,7 +492,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>39264969020.21658</v>
+        <v>39201564034.85326</v>
       </c>
     </row>
     <row r="5">
@@ -507,7 +507,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>33336564002.83117</v>
+        <v>33310656530.94685</v>
       </c>
     </row>
     <row r="6">
@@ -522,7 +522,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>24349065386.73361</v>
+        <v>24399622165.73147</v>
       </c>
     </row>
     <row r="7">
@@ -537,7 +537,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>13663137986.51064</v>
+        <v>13665400136.30362</v>
       </c>
     </row>
     <row r="8">
@@ -552,7 +552,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>11333989505.26704</v>
+        <v>11304976145.07183</v>
       </c>
     </row>
     <row r="9">
@@ -567,7 +567,7 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>9090267401.994192</v>
+        <v>9056483331.556614</v>
       </c>
     </row>
     <row r="10">
@@ -582,7 +582,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>8236026889.612488</v>
+        <v>8260159516.992143</v>
       </c>
     </row>
     <row r="11">
@@ -597,7 +597,7 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>8081851554.837598</v>
+        <v>8084726899.33145</v>
       </c>
     </row>
     <row r="12">
@@ -612,7 +612,7 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>7626351885.505556</v>
+        <v>7632285366.632638</v>
       </c>
     </row>
     <row r="13">
@@ -627,7 +627,7 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>7583153032.951226</v>
+        <v>7618079701.282753</v>
       </c>
     </row>
     <row r="14">
@@ -642,7 +642,7 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>6707523369.361221</v>
+        <v>6698546429.708444</v>
       </c>
     </row>
     <row r="15">
@@ -657,7 +657,7 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>6141272638.352819</v>
+        <v>6132020529.331023</v>
       </c>
     </row>
     <row r="16">
@@ -672,7 +672,7 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>5191027096.528177</v>
+        <v>5186461309.489183</v>
       </c>
     </row>
     <row r="17">
@@ -687,7 +687,7 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>5051464744.905278</v>
+        <v>5048987793.845691</v>
       </c>
     </row>
     <row r="18">
@@ -702,7 +702,7 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>4465801139.945673</v>
+        <v>4465611717.579144</v>
       </c>
     </row>
     <row r="19">
@@ -717,7 +717,7 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>3664513470.983015</v>
+        <v>3658175713.09136</v>
       </c>
     </row>
     <row r="20">
@@ -732,7 +732,7 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>3461681444.843696</v>
+        <v>3461649966.767</v>
       </c>
     </row>
     <row r="21">
@@ -747,7 +747,7 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>3438582604.318887</v>
+        <v>3434662981.505833</v>
       </c>
     </row>
     <row r="22">
@@ -762,7 +762,7 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>3361110819.951435</v>
+        <v>3363821194.031478</v>
       </c>
     </row>
     <row r="23">
@@ -777,7 +777,7 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>3008383163.518763</v>
+        <v>3012735565.923972</v>
       </c>
     </row>
     <row r="24">
@@ -792,7 +792,7 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>2997551953.684832</v>
+        <v>2993198303.274961</v>
       </c>
     </row>
     <row r="25">
@@ -807,7 +807,7 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>2846611419.595122</v>
+        <v>2851150359.793557</v>
       </c>
     </row>
     <row r="26">
@@ -822,7 +822,7 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>2437929453.019127</v>
+        <v>2432964843.350379</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
plot the list of stocks and crypto
</commit_message>
<xml_diff>
--- a/cryptos_market_cap.xlsx
+++ b/cryptos_market_cap.xlsx
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>734283209566.5956</v>
+        <v>732621518415.6881</v>
       </c>
     </row>
     <row r="3">
@@ -477,7 +477,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>245227573040.3853</v>
+        <v>244544162085.86</v>
       </c>
     </row>
     <row r="4">
@@ -492,7 +492,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>39201564034.85326</v>
+        <v>39021256108.05149</v>
       </c>
     </row>
     <row r="5">
@@ -507,7 +507,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>33310656530.94685</v>
+        <v>33240319443.19441</v>
       </c>
     </row>
     <row r="6">
@@ -522,7 +522,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>24399622165.73147</v>
+        <v>24192102645.34322</v>
       </c>
     </row>
     <row r="7">
@@ -537,7 +537,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>13665400136.30362</v>
+        <v>13626977438.05725</v>
       </c>
     </row>
     <row r="8">
@@ -552,7 +552,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>11304976145.07183</v>
+        <v>11276561340.28382</v>
       </c>
     </row>
     <row r="9">
@@ -567,7 +567,7 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>9056483331.556614</v>
+        <v>9044693106.554544</v>
       </c>
     </row>
     <row r="10">
@@ -582,7 +582,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>8260159516.992143</v>
+        <v>8216551625.333233</v>
       </c>
     </row>
     <row r="11">
@@ -597,7 +597,7 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>8084726899.33145</v>
+        <v>7983491076.597414</v>
       </c>
     </row>
     <row r="12">
@@ -612,7 +612,7 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>7632285366.632638</v>
+        <v>7616338019.167827</v>
       </c>
     </row>
     <row r="13">
@@ -627,7 +627,7 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>7618079701.282753</v>
+        <v>7579762307.742823</v>
       </c>
     </row>
     <row r="14">
@@ -642,7 +642,7 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>6698546429.708444</v>
+        <v>6682877131.788206</v>
       </c>
     </row>
     <row r="15">
@@ -657,7 +657,7 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>6132020529.331023</v>
+        <v>6125944627.159385</v>
       </c>
     </row>
     <row r="16">
@@ -672,7 +672,7 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>5186461309.489183</v>
+        <v>5176081409.588452</v>
       </c>
     </row>
     <row r="17">
@@ -687,7 +687,7 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>5048987793.845691</v>
+        <v>5036113315.379909</v>
       </c>
     </row>
     <row r="18">
@@ -702,7 +702,7 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>4465611717.579144</v>
+        <v>4460651036.843834</v>
       </c>
     </row>
     <row r="19">
@@ -717,7 +717,7 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>3658175713.09136</v>
+        <v>3657433322.423396</v>
       </c>
     </row>
     <row r="20">
@@ -732,7 +732,7 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>3461649966.767</v>
+        <v>3446382275.144342</v>
       </c>
     </row>
     <row r="21">
@@ -747,7 +747,7 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>3434662981.505833</v>
+        <v>3425579876.474032</v>
       </c>
     </row>
     <row r="22">
@@ -762,7 +762,7 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>3363821194.031478</v>
+        <v>3352688912.854328</v>
       </c>
     </row>
     <row r="23">
@@ -777,7 +777,7 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>3012735565.923972</v>
+        <v>3006698295.104897</v>
       </c>
     </row>
     <row r="24">
@@ -792,7 +792,7 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>2993198303.274961</v>
+        <v>2975587062.48001</v>
       </c>
     </row>
     <row r="25">
@@ -807,7 +807,7 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>2851150359.793557</v>
+        <v>2833196183.419603</v>
       </c>
     </row>
     <row r="26">
@@ -822,7 +822,7 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>2432964843.350379</v>
+        <v>2432555563.773227</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
FrontEnd : MyPortfolio v2
</commit_message>
<xml_diff>
--- a/cryptos_market_cap.xlsx
+++ b/cryptos_market_cap.xlsx
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>732666015714.3153</v>
+        <v>731328207344.1487</v>
       </c>
     </row>
     <row r="3">
@@ -477,7 +477,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>243390022314.4409</v>
+        <v>243848336462.4445</v>
       </c>
     </row>
     <row r="4">
@@ -492,7 +492,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>38553263308.80518</v>
+        <v>38897308613.14926</v>
       </c>
     </row>
     <row r="5">
@@ -507,7 +507,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>33017420124.65859</v>
+        <v>33031459115.72026</v>
       </c>
     </row>
     <row r="6">
@@ -522,7 +522,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>24045736641.4287</v>
+        <v>24108716716.17286</v>
       </c>
     </row>
     <row r="7">
@@ -537,7 +537,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>13461116528.69757</v>
+        <v>13546617417.9198</v>
       </c>
     </row>
     <row r="8">
@@ -552,7 +552,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>11064839997.36963</v>
+        <v>11110165998.26605</v>
       </c>
     </row>
     <row r="9">
@@ -567,7 +567,7 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>8960583136.712769</v>
+        <v>8995956627.739824</v>
       </c>
     </row>
     <row r="10">
@@ -582,7 +582,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>8092363142.580025</v>
+        <v>8130294178.05073</v>
       </c>
     </row>
     <row r="11">
@@ -597,7 +597,7 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>7988591938.638286</v>
+        <v>8031994567.728826</v>
       </c>
     </row>
     <row r="12">
@@ -612,7 +612,7 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>7520098175.876218</v>
+        <v>7546205033.673535</v>
       </c>
     </row>
     <row r="13">
@@ -627,7 +627,7 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>7422617002.338256</v>
+        <v>7435826137.515828</v>
       </c>
     </row>
     <row r="14">
@@ -642,7 +642,7 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>6867663609.434041</v>
+        <v>6637440630.684655</v>
       </c>
     </row>
     <row r="15">
@@ -657,7 +657,7 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>6084990472.010634</v>
+        <v>6086459300.24696</v>
       </c>
     </row>
     <row r="16">
@@ -672,7 +672,7 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>5148749028.02157</v>
+        <v>5172735273.081258</v>
       </c>
     </row>
     <row r="17">
@@ -687,7 +687,7 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>4983489915.455687</v>
+        <v>4997271780.234427</v>
       </c>
     </row>
     <row r="18">
@@ -702,7 +702,7 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>4434950716.939951</v>
+        <v>4449279246.849122</v>
       </c>
     </row>
     <row r="19">
@@ -717,7 +717,7 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>3658270103.735498</v>
+        <v>3658360719.434418</v>
       </c>
     </row>
     <row r="20">
@@ -732,7 +732,7 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>3452732850.315029</v>
+        <v>3453039002.858096</v>
       </c>
     </row>
     <row r="21">
@@ -747,7 +747,7 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>3378102172.321451</v>
+        <v>3393770849.066844</v>
       </c>
     </row>
     <row r="22">
@@ -762,7 +762,7 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>3355757906.561194</v>
+        <v>3358900876.520487</v>
       </c>
     </row>
     <row r="23">
@@ -777,7 +777,7 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>3002407538.344346</v>
+        <v>3005546425.306632</v>
       </c>
     </row>
     <row r="24">
@@ -792,7 +792,7 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>2819431652.400485</v>
+        <v>2856450754.591782</v>
       </c>
     </row>
     <row r="25">
@@ -807,7 +807,7 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>2812931796.373783</v>
+        <v>2820653867.299805</v>
       </c>
     </row>
     <row r="26">
@@ -822,7 +822,7 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>2411014515.115713</v>
+        <v>2421578972.477175</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
my portoflio css re shape
</commit_message>
<xml_diff>
--- a/cryptos_market_cap.xlsx
+++ b/cryptos_market_cap.xlsx
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>722113178923.26</v>
+        <v>704448480175.6102</v>
       </c>
     </row>
     <row r="3">
@@ -477,7 +477,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>239541254496.6913</v>
+        <v>234301122105.401</v>
       </c>
     </row>
     <row r="4">
@@ -492,7 +492,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>36740641785.06532</v>
+        <v>34780481584.6476</v>
       </c>
     </row>
     <row r="5">
@@ -507,7 +507,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>32191662585.45895</v>
+        <v>31440446351.24937</v>
       </c>
     </row>
     <row r="6">
@@ -522,7 +522,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>23183652184.08698</v>
+        <v>22409126657.29711</v>
       </c>
     </row>
     <row r="7">
@@ -537,7 +537,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>13162405346.01293</v>
+        <v>12771770288.35733</v>
       </c>
     </row>
     <row r="8">
@@ -552,7 +552,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>10689268462.68528</v>
+        <v>10367684249.58487</v>
       </c>
     </row>
     <row r="9">
@@ -567,7 +567,7 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>8655780829.482132</v>
+        <v>8595727131.068867</v>
       </c>
     </row>
     <row r="10">
@@ -582,7 +582,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>8069886228.533433</v>
+        <v>7968598284.179463</v>
       </c>
     </row>
     <row r="11">
@@ -597,7 +597,7 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>7848601797.129404</v>
+        <v>7597837770.961227</v>
       </c>
     </row>
     <row r="12">
@@ -612,7 +612,7 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>7368501427.929321</v>
+        <v>6882296974.000452</v>
       </c>
     </row>
     <row r="13">
@@ -627,7 +627,7 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>7025247575.183109</v>
+        <v>6836765843.319241</v>
       </c>
     </row>
     <row r="14">
@@ -642,7 +642,7 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>6541123252.099557</v>
+        <v>6154115361.756376</v>
       </c>
     </row>
     <row r="15">
@@ -657,7 +657,7 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>6014961546.785239</v>
+        <v>5864055698.012118</v>
       </c>
     </row>
     <row r="16">
@@ -672,7 +672,7 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>5072757524.645171</v>
+        <v>4943884169.308591</v>
       </c>
     </row>
     <row r="17">
@@ -687,7 +687,7 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>4773461099.742822</v>
+        <v>4622630406.286113</v>
       </c>
     </row>
     <row r="18">
@@ -702,7 +702,7 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>4444005031.695962</v>
+        <v>4274405809.596792</v>
       </c>
     </row>
     <row r="19">
@@ -717,7 +717,7 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>3674983780.836744</v>
+        <v>3671686599.97737</v>
       </c>
     </row>
     <row r="20">
@@ -732,7 +732,7 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>3522698948.715496</v>
+        <v>3401380976.234488</v>
       </c>
     </row>
     <row r="21">
@@ -747,7 +747,7 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>3263215983.659451</v>
+        <v>3192916216.664364</v>
       </c>
     </row>
     <row r="22">
@@ -762,7 +762,7 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>3250473474.281646</v>
+        <v>3132420847.329648</v>
       </c>
     </row>
     <row r="23">
@@ -777,37 +777,37 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>2982976949.005098</v>
+        <v>2922229784.867324</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Ethereum Classic</t>
+          <t>Kaspa</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>ETC-USD</t>
+          <t>KAS-USD</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>2725063746.491085</v>
+        <v>2678810291.723003</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Kaspa</t>
+          <t>Ethereum Classic</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>KAS-USD</t>
+          <t>ETC-USD</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>2708848523.561298</v>
+        <v>2632693755.895442</v>
       </c>
     </row>
     <row r="26">
@@ -822,7 +822,7 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>2228026260.7799</v>
+        <v>2193394215.989171</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
css refactor and chnages
</commit_message>
<xml_diff>
--- a/cryptos_market_cap.xlsx
+++ b/cryptos_market_cap.xlsx
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>704448480175.6102</v>
+        <v>713408145429.4626</v>
       </c>
     </row>
     <row r="3">
@@ -477,7 +477,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>234301122105.401</v>
+        <v>242814620310.7914</v>
       </c>
     </row>
     <row r="4">
@@ -492,7 +492,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>34780481584.6476</v>
+        <v>35356419041.60538</v>
       </c>
     </row>
     <row r="5">
@@ -507,7 +507,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>31440446351.24937</v>
+        <v>31952860863.86129</v>
       </c>
     </row>
     <row r="6">
@@ -522,7 +522,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>22409126657.29711</v>
+        <v>23219394016.70679</v>
       </c>
     </row>
     <row r="7">
@@ -537,7 +537,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>12771770288.35733</v>
+        <v>13054128698.86161</v>
       </c>
     </row>
     <row r="8">
@@ -552,7 +552,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>10367684249.58487</v>
+        <v>10572957351.13158</v>
       </c>
     </row>
     <row r="9">
@@ -567,7 +567,7 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>8595727131.068867</v>
+        <v>8855656019.970976</v>
       </c>
     </row>
     <row r="10">
@@ -582,7 +582,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>7968598284.179463</v>
+        <v>8207533770.940097</v>
       </c>
     </row>
     <row r="11">
@@ -597,7 +597,7 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>7597837770.961227</v>
+        <v>7899877325.028001</v>
       </c>
     </row>
     <row r="12">
@@ -612,7 +612,7 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>6882296974.000452</v>
+        <v>7172856209.641662</v>
       </c>
     </row>
     <row r="13">
@@ -627,7 +627,7 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>6836765843.319241</v>
+        <v>7052109471.634726</v>
       </c>
     </row>
     <row r="14">
@@ -642,7 +642,7 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>6154115361.756376</v>
+        <v>6549647879.810579</v>
       </c>
     </row>
     <row r="15">
@@ -657,7 +657,7 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>5864055698.012118</v>
+        <v>5943020494.124944</v>
       </c>
     </row>
     <row r="16">
@@ -672,7 +672,7 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>4943884169.308591</v>
+        <v>5001855713.450159</v>
       </c>
     </row>
     <row r="17">
@@ -687,7 +687,7 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>4622630406.286113</v>
+        <v>4696164014.753898</v>
       </c>
     </row>
     <row r="18">
@@ -702,7 +702,7 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>4274405809.596792</v>
+        <v>4300199471.765975</v>
       </c>
     </row>
     <row r="19">
@@ -717,7 +717,7 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>3671686599.97737</v>
+        <v>3734294537.424081</v>
       </c>
     </row>
     <row r="20">
@@ -732,7 +732,7 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>3401380976.234488</v>
+        <v>3461093890.421829</v>
       </c>
     </row>
     <row r="21">
@@ -747,7 +747,7 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>3192916216.664364</v>
+        <v>3254968381.180032</v>
       </c>
     </row>
     <row r="22">
@@ -762,7 +762,7 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>3132420847.329648</v>
+        <v>3233171860.471212</v>
       </c>
     </row>
     <row r="23">
@@ -777,7 +777,7 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>2922229784.867324</v>
+        <v>2978080122.785878</v>
       </c>
     </row>
     <row r="24">
@@ -792,7 +792,7 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>2678810291.723003</v>
+        <v>2855259008.35902</v>
       </c>
     </row>
     <row r="25">
@@ -807,7 +807,7 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>2632693755.895442</v>
+        <v>2685551641.418438</v>
       </c>
     </row>
     <row r="26">
@@ -822,7 +822,7 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>2193394215.989171</v>
+        <v>2406688509.304906</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New routes, return error
</commit_message>
<xml_diff>
--- a/cryptos_market_cap.xlsx
+++ b/cryptos_market_cap.xlsx
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>723664642022.0618</v>
+        <v>728127757485.9529</v>
       </c>
     </row>
     <row r="3">
@@ -477,7 +477,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>246758836044.4923</v>
+        <v>248947206859.0277</v>
       </c>
     </row>
     <row r="4">
@@ -492,7 +492,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>35529898585.5086</v>
+        <v>35842103923.58646</v>
       </c>
     </row>
     <row r="5">
@@ -507,7 +507,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>32399619081.34889</v>
+        <v>32789094089.75835</v>
       </c>
     </row>
     <row r="6">
@@ -522,7 +522,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>23664223911.57412</v>
+        <v>24185017211.16008</v>
       </c>
     </row>
     <row r="7">
@@ -537,7 +537,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>13219991303.29176</v>
+        <v>13352606143.86956</v>
       </c>
     </row>
     <row r="8">
@@ -552,7 +552,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>10739918741.23616</v>
+        <v>10759940815.95023</v>
       </c>
     </row>
     <row r="9">
@@ -567,7 +567,7 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>8927731083.832275</v>
+        <v>8966284996.765963</v>
       </c>
     </row>
     <row r="10">
@@ -582,7 +582,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>8276582658.967429</v>
+        <v>8292017669.368899</v>
       </c>
     </row>
     <row r="11">
@@ -597,7 +597,7 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>8012707389.134512</v>
+        <v>8086467521.47689</v>
       </c>
     </row>
     <row r="12">
@@ -612,7 +612,7 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>7238815020.729666</v>
+        <v>7532202354.016511</v>
       </c>
     </row>
     <row r="13">
@@ -627,7 +627,7 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>7123434403.883887</v>
+        <v>7190147621.414537</v>
       </c>
     </row>
     <row r="14">
@@ -642,7 +642,7 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>6720402596.581711</v>
+        <v>6789191812.222837</v>
       </c>
     </row>
     <row r="15">
@@ -657,7 +657,7 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>5987551062.269527</v>
+        <v>6059270581.208712</v>
       </c>
     </row>
     <row r="16">
@@ -672,7 +672,7 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>5044062020.346442</v>
+        <v>5056212888.394469</v>
       </c>
     </row>
     <row r="17">
@@ -687,7 +687,7 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>4738421330.108534</v>
+        <v>4774750034.886718</v>
       </c>
     </row>
     <row r="18">
@@ -702,7 +702,7 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>4317735068.687028</v>
+        <v>4361698573.192698</v>
       </c>
     </row>
     <row r="19">
@@ -717,7 +717,7 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>3729676728.043265</v>
+        <v>3757389910.898662</v>
       </c>
     </row>
     <row r="20">
@@ -732,7 +732,7 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>3473936263.348656</v>
+        <v>3492021508.260048</v>
       </c>
     </row>
     <row r="21">
@@ -747,7 +747,7 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>3308787905.137556</v>
+        <v>3330599207.781488</v>
       </c>
     </row>
     <row r="22">
@@ -762,7 +762,7 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>3276888163.457403</v>
+        <v>3300542812.614562</v>
       </c>
     </row>
     <row r="23">
@@ -777,7 +777,7 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>2997442898.587745</v>
+        <v>2999817564.762733</v>
       </c>
     </row>
     <row r="24">
@@ -792,7 +792,7 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>2797612208.228825</v>
+        <v>2847168829.225609</v>
       </c>
     </row>
     <row r="25">
@@ -807,7 +807,7 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>2723694050.90598</v>
+        <v>2750220253.895219</v>
       </c>
     </row>
     <row r="26">
@@ -822,7 +822,7 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>2381182584.020131</v>
+        <v>2392904552.53546</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
beta and fucking alpha
</commit_message>
<xml_diff>
--- a/cryptos_market_cap.xlsx
+++ b/cryptos_market_cap.xlsx
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>728127757485.9529</v>
+        <v>729452307914.964</v>
       </c>
     </row>
     <row r="3">
@@ -477,7 +477,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>248947206859.0277</v>
+        <v>247274651738.1406</v>
       </c>
     </row>
     <row r="4">
@@ -492,7 +492,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>35842103923.58646</v>
+        <v>35889246967.43371</v>
       </c>
     </row>
     <row r="5">
@@ -507,7 +507,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>32789094089.75835</v>
+        <v>32841118931.31339</v>
       </c>
     </row>
     <row r="6">
@@ -522,7 +522,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>24185017211.16008</v>
+        <v>24437405375.18588</v>
       </c>
     </row>
     <row r="7">
@@ -537,7 +537,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>13352606143.86956</v>
+        <v>13445294161.80837</v>
       </c>
     </row>
     <row r="8">
@@ -552,7 +552,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>10759940815.95023</v>
+        <v>10773844725.77612</v>
       </c>
     </row>
     <row r="9">
@@ -567,7 +567,7 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>8966284996.765963</v>
+        <v>8984553336.742424</v>
       </c>
     </row>
     <row r="10">
@@ -582,7 +582,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>8292017669.368899</v>
+        <v>8235606022.197677</v>
       </c>
     </row>
     <row r="11">
@@ -597,7 +597,7 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>8086467521.47689</v>
+        <v>8035539860.119489</v>
       </c>
     </row>
     <row r="12">
@@ -612,7 +612,7 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>7532202354.016511</v>
+        <v>7438036117.054225</v>
       </c>
     </row>
     <row r="13">
@@ -627,7 +627,7 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>7190147621.414537</v>
+        <v>7192503295.905393</v>
       </c>
     </row>
     <row r="14">
@@ -642,7 +642,7 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>6789191812.222837</v>
+        <v>6462221783.156593</v>
       </c>
     </row>
     <row r="15">
@@ -657,7 +657,7 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>6059270581.208712</v>
+        <v>6071707533.534866</v>
       </c>
     </row>
     <row r="16">
@@ -672,7 +672,7 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>5056212888.394469</v>
+        <v>5110220791.4047</v>
       </c>
     </row>
     <row r="17">
@@ -687,7 +687,7 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>4774750034.886718</v>
+        <v>4795370539.839595</v>
       </c>
     </row>
     <row r="18">
@@ -702,7 +702,7 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>4361698573.192698</v>
+        <v>4412458485.5137</v>
       </c>
     </row>
     <row r="19">
@@ -717,7 +717,7 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>3757389910.898662</v>
+        <v>3792471051.095762</v>
       </c>
     </row>
     <row r="20">
@@ -732,7 +732,7 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>3492021508.260048</v>
+        <v>3489926144.652276</v>
       </c>
     </row>
     <row r="21">
@@ -747,7 +747,7 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>3330599207.781488</v>
+        <v>3322514833.25357</v>
       </c>
     </row>
     <row r="22">
@@ -762,7 +762,7 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>3300542812.614562</v>
+        <v>3306057057.413295</v>
       </c>
     </row>
     <row r="23">
@@ -777,37 +777,37 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>2999817564.762733</v>
+        <v>3007520499.669557</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Kaspa</t>
+          <t>Ethereum Classic</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>KAS-USD</t>
+          <t>ETC-USD</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>2847168829.225609</v>
+        <v>2732922419.353358</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Ethereum Classic</t>
+          <t>Kaspa</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>ETC-USD</t>
+          <t>KAS-USD</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>2750220253.895219</v>
+        <v>2730235727.597404</v>
       </c>
     </row>
     <row r="26">
@@ -822,7 +822,7 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>2392904552.53546</v>
+        <v>2474737191.456425</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add to portoflio route
</commit_message>
<xml_diff>
--- a/cryptos_market_cap.xlsx
+++ b/cryptos_market_cap.xlsx
@@ -91,12 +91,12 @@
     <t>Monero</t>
   </si>
   <si>
+    <t>Ethereum Classic</t>
+  </si>
+  <si>
     <t>Kaspa</t>
   </si>
   <si>
-    <t>Ethereum Classic</t>
-  </si>
-  <si>
     <t>Cronos</t>
   </si>
   <si>
@@ -166,10 +166,10 @@
     <t>XMR-USD</t>
   </si>
   <si>
+    <t>ETC-USD</t>
+  </si>
+  <si>
     <t>KAS-USD</t>
-  </si>
-  <si>
-    <t>ETC-USD</t>
   </si>
   <si>
     <t>CRO-USD</t>
@@ -555,7 +555,7 @@
         <v>28</v>
       </c>
       <c r="C2">
-        <v>731801244153.6709</v>
+        <v>722372549397.9398</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -566,7 +566,7 @@
         <v>29</v>
       </c>
       <c r="C3">
-        <v>248007068333.1828</v>
+        <v>245521447938.1596</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -577,7 +577,7 @@
         <v>30</v>
       </c>
       <c r="C4">
-        <v>35395418901.69009</v>
+        <v>35021155768.29485</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -588,7 +588,7 @@
         <v>31</v>
       </c>
       <c r="C5">
-        <v>33020921140.4625</v>
+        <v>33120120499.31993</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -599,7 +599,7 @@
         <v>32</v>
       </c>
       <c r="C6">
-        <v>24706903066.42802</v>
+        <v>23975012550.49981</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -610,7 +610,7 @@
         <v>33</v>
       </c>
       <c r="C7">
-        <v>13575901748.9755</v>
+        <v>13351213137.83818</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -621,7 +621,7 @@
         <v>34</v>
       </c>
       <c r="C8">
-        <v>10766599426.3989</v>
+        <v>10669931425.47692</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -632,7 +632,7 @@
         <v>35</v>
       </c>
       <c r="C9">
-        <v>8979805351.594442</v>
+        <v>8951670740.955879</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -643,7 +643,7 @@
         <v>36</v>
       </c>
       <c r="C10">
-        <v>8228914821.425825</v>
+        <v>8152034859.065285</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -654,7 +654,7 @@
         <v>37</v>
       </c>
       <c r="C11">
-        <v>7988891072.718956</v>
+        <v>7896231715.013188</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -665,7 +665,7 @@
         <v>38</v>
       </c>
       <c r="C12">
-        <v>7505122373.168587</v>
+        <v>7334370645.503334</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -676,7 +676,7 @@
         <v>39</v>
       </c>
       <c r="C13">
-        <v>7204323880.560933</v>
+        <v>7108959453.460295</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -687,7 +687,7 @@
         <v>40</v>
       </c>
       <c r="C14">
-        <v>6448275294.744733</v>
+        <v>6375380161.262115</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -698,7 +698,7 @@
         <v>41</v>
       </c>
       <c r="C15">
-        <v>6082546680.400978</v>
+        <v>6029360761.003362</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -709,7 +709,7 @@
         <v>42</v>
       </c>
       <c r="C16">
-        <v>5118735412.930139</v>
+        <v>5072080315.086798</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -720,7 +720,7 @@
         <v>43</v>
       </c>
       <c r="C17">
-        <v>4786772408.724358</v>
+        <v>4729853488.20554</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -731,7 +731,7 @@
         <v>44</v>
       </c>
       <c r="C18">
-        <v>4402570246.135977</v>
+        <v>4362049864.072336</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -742,7 +742,7 @@
         <v>45</v>
       </c>
       <c r="C19">
-        <v>3811696996.905764</v>
+        <v>3790164544.140406</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -753,7 +753,7 @@
         <v>46</v>
       </c>
       <c r="C20">
-        <v>3524737138.645567</v>
+        <v>3452298824.828917</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -764,7 +764,7 @@
         <v>47</v>
       </c>
       <c r="C21">
-        <v>3358985683.710223</v>
+        <v>3271220148.296094</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -775,7 +775,7 @@
         <v>48</v>
       </c>
       <c r="C22">
-        <v>3289468847.247729</v>
+        <v>3260350550.203758</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -786,7 +786,7 @@
         <v>49</v>
       </c>
       <c r="C23">
-        <v>3054187170.113299</v>
+        <v>3044044602.572844</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -797,7 +797,7 @@
         <v>50</v>
       </c>
       <c r="C24">
-        <v>2811695940.43936</v>
+        <v>2703391028.716319</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -808,7 +808,7 @@
         <v>51</v>
       </c>
       <c r="C25">
-        <v>2740147031.053804</v>
+        <v>2690569435.013835</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -819,7 +819,7 @@
         <v>52</v>
       </c>
       <c r="C26">
-        <v>2376592054.92052</v>
+        <v>2314128781.164953</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
buf fixing for alphas and betas
</commit_message>
<xml_diff>
--- a/cryptos_market_cap.xlsx
+++ b/cryptos_market_cap.xlsx
@@ -555,7 +555,7 @@
         <v>28</v>
       </c>
       <c r="C2">
-        <v>726136673782.9392</v>
+        <v>728468337064.214</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -566,7 +566,7 @@
         <v>29</v>
       </c>
       <c r="C3">
-        <v>246739776141.3557</v>
+        <v>247582345045.7819</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -577,7 +577,7 @@
         <v>30</v>
       </c>
       <c r="C4">
-        <v>35232503409.22829</v>
+        <v>35258720994.39204</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -588,7 +588,7 @@
         <v>31</v>
       </c>
       <c r="C5">
-        <v>33095194768.09108</v>
+        <v>33256557461.85886</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -599,7 +599,7 @@
         <v>32</v>
       </c>
       <c r="C6">
-        <v>24058640939.11256</v>
+        <v>24029275225.26164</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -610,7 +610,7 @@
         <v>33</v>
       </c>
       <c r="C7">
-        <v>13462976480.86654</v>
+        <v>13494726670.04683</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -621,7 +621,7 @@
         <v>34</v>
       </c>
       <c r="C8">
-        <v>10726470819.17894</v>
+        <v>10773566732.13237</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -632,7 +632,7 @@
         <v>35</v>
       </c>
       <c r="C9">
-        <v>8966599330.80106</v>
+        <v>9012306940.781408</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -643,7 +643,7 @@
         <v>36</v>
       </c>
       <c r="C10">
-        <v>8234328670.67699</v>
+        <v>8298860851.393289</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -654,7 +654,7 @@
         <v>37</v>
       </c>
       <c r="C11">
-        <v>7925892764.690978</v>
+        <v>8107879007.03618</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -665,7 +665,7 @@
         <v>38</v>
       </c>
       <c r="C12">
-        <v>7407753876.200377</v>
+        <v>7358767498.515913</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -676,7 +676,7 @@
         <v>39</v>
       </c>
       <c r="C13">
-        <v>7152603693.07559</v>
+        <v>7212440177.912173</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -687,7 +687,7 @@
         <v>40</v>
       </c>
       <c r="C14">
-        <v>6403599015.264664</v>
+        <v>6662263144.838155</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -698,7 +698,7 @@
         <v>41</v>
       </c>
       <c r="C15">
-        <v>6034448458.853427</v>
+        <v>6051715601.171719</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -709,7 +709,7 @@
         <v>42</v>
       </c>
       <c r="C16">
-        <v>5102206036.627727</v>
+        <v>5127222348.481926</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -720,7 +720,7 @@
         <v>43</v>
       </c>
       <c r="C17">
-        <v>4752616482.879973</v>
+        <v>4765344038.656413</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -731,7 +731,7 @@
         <v>44</v>
       </c>
       <c r="C18">
-        <v>4376733596.606018</v>
+        <v>4401359373.274726</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -742,7 +742,7 @@
         <v>45</v>
       </c>
       <c r="C19">
-        <v>3784373046.235852</v>
+        <v>3778981678.160348</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -753,7 +753,7 @@
         <v>46</v>
       </c>
       <c r="C20">
-        <v>3456925992.065712</v>
+        <v>3487123027.636964</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -764,7 +764,7 @@
         <v>47</v>
       </c>
       <c r="C21">
-        <v>3288333466.37686</v>
+        <v>3293326415.479542</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -775,7 +775,7 @@
         <v>48</v>
       </c>
       <c r="C22">
-        <v>3267917456.664171</v>
+        <v>3275289772.452466</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -786,7 +786,7 @@
         <v>49</v>
       </c>
       <c r="C23">
-        <v>3054998441.419912</v>
+        <v>3054902357.104695</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -797,7 +797,7 @@
         <v>50</v>
       </c>
       <c r="C24">
-        <v>2728344596.269171</v>
+        <v>2777804281.923453</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -808,7 +808,7 @@
         <v>51</v>
       </c>
       <c r="C25">
-        <v>2713033976.980379</v>
+        <v>2721418246.808467</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -819,7 +819,7 @@
         <v>52</v>
       </c>
       <c r="C26">
-        <v>2326377962.078745</v>
+        <v>2361333413.99097</v>
       </c>
     </row>
   </sheetData>

</xml_diff>